<commit_message>
se agrega el script para crear la base de datos
</commit_message>
<xml_diff>
--- a/src/main/resources/static/boceto-bd/base-de-datos.xlsx
+++ b/src/main/resources/static/boceto-bd/base-de-datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0fb8f5a7c6acabee/INSPT/2do Año/Programacion 2/12 - Final con Spring/Holding-Management/src/main/resources/static/boceto-bd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{735BE250-E3C6-418B-BAB2-8B90942BEB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB72D714-844A-462A-AFEB-E42FDEC2C95C}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{735BE250-E3C6-418B-BAB2-8B90942BEB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EFF437A-8CA6-4B5B-BCED-C23B4086896E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{2BCF5C3B-BEE5-45D2-93E7-6698EF6AA72D}"/>
   </bookViews>
@@ -225,11 +225,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -240,10 +242,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -563,7 +561,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,10 +616,10 @@
       <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -630,7 +628,7 @@
       <c r="K2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="1" t="s">
         <v>31</v>
       </c>
       <c r="M2" s="2"/>
@@ -665,7 +663,7 @@
       <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -705,7 +703,7 @@
       <c r="E8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J8" s="1" t="s">
@@ -727,7 +725,7 @@
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="9"/>
+      <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -737,9 +735,9 @@
         <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J11" s="1" t="s">
@@ -751,7 +749,6 @@
       <c r="L11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M11" s="8"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -775,7 +772,7 @@
       <c r="C14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J14" s="1" t="s">

</xml_diff>